<commit_message>
updating h1 to .h1
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Builds\dashboardv.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182B9FB0-EFE7-4025-945A-56A4C99462B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEE000B-3665-470E-8650-00E374A85EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,11 @@
     <sheet name="2014" sheetId="3" r:id="rId1"/>
     <sheet name="2015" sheetId="4" r:id="rId2"/>
     <sheet name="2016" sheetId="6" r:id="rId3"/>
-    <sheet name="2024" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Table3" localSheetId="0">#REF!</definedName>
     <definedName name="Table3" localSheetId="1">#REF!</definedName>
     <definedName name="Table3" localSheetId="2">#REF!</definedName>
-    <definedName name="Table3" localSheetId="3">#REF!</definedName>
     <definedName name="Table3">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -80,10 +78,6 @@
   </si>
   <si>
     <t>Manara Content</t>
-  </si>
-  <si>
-    <t>2024 Year Resolution As a 32-Year-Old
-Is To Learn Egypt Course Content For Programming</t>
   </si>
   <si>
     <t>Done</t>
@@ -326,106 +320,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <b val="0"/>
@@ -737,52 +632,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F99927F6-9A86-4551-901E-A1F9F7A952FA}" name="Table57815" displayName="Table57815" ref="A4:D163" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{F99927F6-9A86-4551-901E-A1F9F7A952FA}" name="Table57815" displayName="Table57815" ref="A4:D163" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A4:D163" xr:uid="{D6433E5E-10F4-4533-AA28-A0287449AC3B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D7D35201-009C-416A-A1A1-DBB870305BE1}" name="Date" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{1B5A8BBB-C29E-40A7-B4FC-A79F8485AB7A}" name="FROM" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{A9247F69-44F9-4794-A15C-435B97974587}" name="TO" dataDxfId="19" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{6C00565E-D97D-42F1-BB1C-4AF2276E6622}" name="CHECK" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{D7D35201-009C-416A-A1A1-DBB870305BE1}" name="Date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{1B5A8BBB-C29E-40A7-B4FC-A79F8485AB7A}" name="FROM" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{A9247F69-44F9-4794-A15C-435B97974587}" name="TO" dataDxfId="13" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{6C00565E-D97D-42F1-BB1C-4AF2276E6622}" name="CHECK" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FCC2F6CE-60DD-4379-9086-A6FEDF28FFC3}" name="Table578159" displayName="Table578159" ref="A4:D369" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FCC2F6CE-60DD-4379-9086-A6FEDF28FFC3}" name="Table578159" displayName="Table578159" ref="A4:D369" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A4:D369" xr:uid="{D6433E5E-10F4-4533-AA28-A0287449AC3B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6E873468-4B14-4EC9-8094-E931DC7A4F38}" name="Date" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{DDECA2C1-13BD-4970-97A6-53CC368AFF58}" name="FROM" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{5A30831E-C9FF-4BAD-88AA-01CE518426D3}" name="TO" dataDxfId="13" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{D7275E59-04C9-40FA-8C8C-24A1864ED81A}" name="CHECK" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{6E873468-4B14-4EC9-8094-E931DC7A4F38}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{DDECA2C1-13BD-4970-97A6-53CC368AFF58}" name="FROM" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{5A30831E-C9FF-4BAD-88AA-01CE518426D3}" name="TO" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{D7275E59-04C9-40FA-8C8C-24A1864ED81A}" name="CHECK" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88E32ADD-C525-4B24-94AF-6FF2156B13EB}" name="Table5781592" displayName="Table5781592" ref="A4:D369" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88E32ADD-C525-4B24-94AF-6FF2156B13EB}" name="Table5781592" displayName="Table5781592" ref="A4:D369" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A4:D369" xr:uid="{D6433E5E-10F4-4533-AA28-A0287449AC3B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4D04A998-DB4B-4826-9195-4A07D47CD1A2}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{2DEDE059-F570-44B3-A231-A3DD97041A88}" name="FROM" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{46937CAC-4FF9-41CB-B2FF-02CD072E8E93}" name="TO" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{21A6BA59-195D-495B-A8CC-26E6359433DF}" name="CHECK" dataDxfId="6"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6D9CE4CB-7343-428D-9C95-00C8AF5C624B}" name="Table57815910" displayName="Table57815910" ref="A4:D163" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A4:D163" xr:uid="{D6433E5E-10F4-4533-AA28-A0287449AC3B}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E9E40A68-8B82-4CD2-B8FC-0C43FEDA1EE0}" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{AE68223C-76F8-4C48-B65B-536276E248CC}" name="FROM" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{6BAB6871-833B-4399-9344-8B1A45F447B7}" name="TO" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{D75D02C0-5996-458A-9D1C-81BF50E6E48B}" name="CHECK" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4D04A998-DB4B-4826-9195-4A07D47CD1A2}" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{2DEDE059-F570-44B3-A231-A3DD97041A88}" name="FROM" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{46937CAC-4FF9-41CB-B2FF-02CD072E8E93}" name="TO" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{21A6BA59-195D-495B-A8CC-26E6359433DF}" name="CHECK" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4419,7 +4301,7 @@
         <v>2.4305555555555556E-3</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="14">
         <v>3</v>
@@ -4440,7 +4322,7 @@
         <v>3.004861111111111</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="14">
         <v>3</v>
@@ -4461,7 +4343,7 @@
         <v>7.2916666666661004E-3</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="14">
         <v>3</v>
@@ -4482,7 +4364,7 @@
         <v>9.7222222222213706E-3</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="14">
         <v>3</v>
@@ -4503,7 +4385,7 @@
         <v>1.21527777777766E-2</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="14">
         <v>3</v>
@@ -4524,7 +4406,7 @@
         <v>1.4583333333331901E-2</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="14">
         <v>3</v>
@@ -4545,7 +4427,7 @@
         <v>1.7013888888887201E-2</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="14">
         <v>3</v>
@@ -4566,7 +4448,7 @@
         <v>1.9444444444442498E-2</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="14">
         <v>3</v>
@@ -4587,7 +4469,7 @@
         <v>2.1874999999997799E-2</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="14">
         <v>3</v>
@@ -4608,7 +4490,7 @@
         <v>2.4305555555552999E-2</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="14">
         <v>3</v>
@@ -9829,8 +9711,8 @@
   <dimension ref="A1:H370"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -9844,7 +9726,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -9854,7 +9736,7 @@
     </row>
     <row r="2" spans="1:6" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -9873,11 +9755,11 @@
       <c r="D3" s="23"/>
       <c r="E3" s="5">
         <f ca="1">(E4+(F4/60))/60</f>
-        <v>0.69444444444444453</v>
+        <v>0.80555555555555547</v>
       </c>
       <c r="F3" s="6">
         <f ca="1">(E4+(F4/60))</f>
-        <v>41.666666666666671</v>
+        <v>48.333333333333329</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -9895,11 +9777,11 @@
       </c>
       <c r="E4" s="7">
         <f ca="1">SUMIF(Table5781592[CHECK],"Done",E$5:E$72)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F4" s="7">
         <f ca="1">SUMIF(Table5781592[CHECK],"Done",F$5:F$72)</f>
-        <v>1000</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9913,7 +9795,7 @@
         <v>1.1574074074074073E-3</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="14">
         <v>1</v>
@@ -9934,7 +9816,7 @@
         <v>3.0023148148148149</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="14">
         <v>1</v>
@@ -9955,7 +9837,7 @@
         <v>3.4722222222222901E-3</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="14">
         <v>1</v>
@@ -9976,7 +9858,7 @@
         <v>4.62962962962973E-3</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="14">
         <v>1</v>
@@ -9997,7 +9879,7 @@
         <v>5.7870370370371703E-3</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="14">
         <v>1</v>
@@ -10018,7 +9900,7 @@
         <v>6.9444444444446097E-3</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="14">
         <v>1</v>
@@ -10039,7 +9921,7 @@
         <v>8.1018518518520492E-3</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="14">
         <v>1</v>
@@ -10060,7 +9942,7 @@
         <v>9.2592592592594895E-3</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="14">
         <v>1</v>
@@ -10081,7 +9963,7 @@
         <v>1.04166666666669E-2</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="14">
         <v>1</v>
@@ -10102,7 +9984,7 @@
         <v>1.15740740740744E-2</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="14">
         <v>1</v>
@@ -10123,7 +10005,7 @@
         <v>1.27314814814818E-2</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="14">
         <v>1</v>
@@ -10144,7 +10026,7 @@
         <v>1.38888888888892E-2</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="14">
         <v>1</v>
@@ -10165,7 +10047,7 @@
         <v>1.50462962962967E-2</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="14">
         <v>1</v>
@@ -10186,7 +10068,7 @@
         <v>1.6203703703704098E-2</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="14">
         <v>1</v>
@@ -10207,7 +10089,7 @@
         <v>1.7361111111111601E-2</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="14">
         <v>1</v>
@@ -10228,7 +10110,7 @@
         <v>1.8518518518519E-2</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" s="14">
         <v>1</v>
@@ -10249,7 +10131,7 @@
         <v>1.9675925925926398E-2</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="14">
         <v>1</v>
@@ -10270,7 +10152,7 @@
         <v>2.0833333333333901E-2</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" s="14">
         <v>1</v>
@@ -10291,7 +10173,7 @@
         <v>2.19907407407413E-2</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" s="14">
         <v>1</v>
@@ -10312,7 +10194,7 @@
         <v>2.3148148148148799E-2</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="14">
         <v>1</v>
@@ -10333,7 +10215,7 @@
         <v>2.4305555555556201E-2</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" s="14">
         <v>1</v>
@@ -10354,7 +10236,7 @@
         <v>2.54629629629636E-2</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26" s="14">
         <v>1</v>
@@ -10375,7 +10257,7 @@
         <v>2.6620370370371099E-2</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27" s="14">
         <v>1</v>
@@ -10396,7 +10278,7 @@
         <v>2.7777777777778501E-2</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28" s="14">
         <v>1</v>
@@ -10417,7 +10299,7 @@
         <v>2.8935185185186001E-2</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E29" s="14">
         <v>1</v>
@@ -10437,9 +10319,15 @@
       <c r="C30" s="1">
         <v>3.0092592592593399E-2</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="2"/>
+      <c r="D30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="14">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17">
@@ -10452,9 +10340,15 @@
       <c r="C31" s="1">
         <v>3.1250000000000798E-2</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="2"/>
+      <c r="D31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="14">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17">
@@ -10467,9 +10361,15 @@
       <c r="C32" s="1">
         <v>3.2407407407408301E-2</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="2"/>
+      <c r="D32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="14">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17">
@@ -10482,9 +10382,15 @@
       <c r="C33" s="1">
         <v>3.3564814814815699E-2</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="2"/>
+      <c r="D33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="14">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17">
@@ -15562,2587 +15468,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731FFE7A-F92E-47F8-9055-E3EE479F5F24}">
-  <dimension ref="A1:H175"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="42.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.6640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="1:6" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="5">
-        <f ca="1">(E4+(F4/60))/60</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <f ca="1">(E4+(F4/60))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="7">
-        <f ca="1">SUMIF(Table57815910[CHECK],"Done",E$5:E$72)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
-        <f ca="1">SUMIF(Table57815910[CHECK],"Done",F$5:F$72)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13">
-        <v>42005</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.0416666666666667E-3</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13">
-        <f>A5+1</f>
-        <v>42006</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.0416666666666667E-3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3.0020833333333332</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13">
-        <f t="shared" ref="A7:A70" si="0">A6+1</f>
-        <v>42007</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2.0833333333333298E-3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3.12499999999988E-3</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13">
-        <f t="shared" si="0"/>
-        <v>42008</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3.1250000000000002E-3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.1666666666664897E-3</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13">
-        <f t="shared" si="0"/>
-        <v>42009</v>
-      </c>
-      <c r="B9" s="1">
-        <v>4.1666666666666701E-3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5.2083333333330997E-3</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13">
-        <f t="shared" si="0"/>
-        <v>42010</v>
-      </c>
-      <c r="B10" s="1">
-        <v>5.2083333333333296E-3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>6.2499999999997098E-3</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13">
-        <f t="shared" si="0"/>
-        <v>42011</v>
-      </c>
-      <c r="B11" s="1">
-        <v>6.2500000000000003E-3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>7.2916666666663103E-3</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13">
-        <f t="shared" si="0"/>
-        <v>42012</v>
-      </c>
-      <c r="B12" s="1">
-        <v>7.2916666666666703E-3</v>
-      </c>
-      <c r="C12" s="1">
-        <v>8.3333333333329204E-3</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13">
-        <f t="shared" si="0"/>
-        <v>42013</v>
-      </c>
-      <c r="B13" s="1">
-        <v>8.3333333333333297E-3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>9.3749999999995295E-3</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13">
-        <f t="shared" si="0"/>
-        <v>42014</v>
-      </c>
-      <c r="B14" s="1">
-        <v>9.3749999999999997E-3</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1.0416666666666101E-2</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13">
-        <f t="shared" si="0"/>
-        <v>42015</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.0416666666666701E-2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1.14583333333328E-2</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13">
-        <f t="shared" si="0"/>
-        <v>42016</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1.14583333333333E-2</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1.24999999999994E-2</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="13">
-        <f t="shared" si="0"/>
-        <v>42017</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1.3541666666665999E-2</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13">
-        <f t="shared" si="0"/>
-        <v>42018</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1.35416666666667E-2</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1.45833333333326E-2</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13">
-        <f t="shared" si="0"/>
-        <v>42019</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1.4583333333333301E-2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1.56249999999992E-2</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13">
-        <f t="shared" si="0"/>
-        <v>42020</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1.6666666666665799E-2</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13">
-        <f t="shared" si="0"/>
-        <v>42021</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1.6666666666666701E-2</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1.77083333333324E-2</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13">
-        <f t="shared" si="0"/>
-        <v>42022</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1.7708333333333302E-2</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1.8749999999999E-2</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13">
-        <f t="shared" si="0"/>
-        <v>42023</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1.8749999999999999E-2</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1.9791666666665601E-2</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13">
-        <f t="shared" si="0"/>
-        <v>42024</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.97916666666667E-2</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2.0833333333332201E-2</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13">
-        <f t="shared" si="0"/>
-        <v>42025</v>
-      </c>
-      <c r="B25" s="1">
-        <v>2.0833333333333301E-2</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2.1874999999998802E-2</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13">
-        <f t="shared" si="0"/>
-        <v>42026</v>
-      </c>
-      <c r="B26" s="1">
-        <v>2.1874999999999999E-2</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2.2916666666665499E-2</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13">
-        <f t="shared" si="0"/>
-        <v>42027</v>
-      </c>
-      <c r="B27" s="1">
-        <v>2.29166666666667E-2</v>
-      </c>
-      <c r="C27" s="1">
-        <v>2.39583333333321E-2</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13">
-        <f t="shared" si="0"/>
-        <v>42028</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2.39583333333333E-2</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2.49999999999987E-2</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13">
-        <f t="shared" si="0"/>
-        <v>42029</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2.6041666666665301E-2</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13">
-        <f t="shared" si="0"/>
-        <v>42030</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2.6041666666666699E-2</v>
-      </c>
-      <c r="C30" s="1">
-        <v>2.7083333333331901E-2</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13">
-        <f t="shared" si="0"/>
-        <v>42031</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2.70833333333333E-2</v>
-      </c>
-      <c r="C31" s="1">
-        <v>2.8124999999998498E-2</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13">
-        <f t="shared" si="0"/>
-        <v>42032</v>
-      </c>
-      <c r="B32" s="1">
-        <v>2.8125000000000001E-2</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2.9166666666665099E-2</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13">
-        <f t="shared" si="0"/>
-        <v>42033</v>
-      </c>
-      <c r="B33" s="1">
-        <v>2.9166666666666698E-2</v>
-      </c>
-      <c r="C33" s="1">
-        <v>3.0208333333331699E-2</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="13">
-        <f t="shared" si="0"/>
-        <v>42034</v>
-      </c>
-      <c r="B34" s="1">
-        <v>3.0208333333333299E-2</v>
-      </c>
-      <c r="C34" s="1">
-        <v>3.12499999999983E-2</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13">
-        <f t="shared" si="0"/>
-        <v>42035</v>
-      </c>
-      <c r="B35" s="1">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C35" s="1">
-        <v>3.22916666666649E-2</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="13">
-        <f t="shared" si="0"/>
-        <v>42036</v>
-      </c>
-      <c r="B36" s="1">
-        <v>3.2291666666666698E-2</v>
-      </c>
-      <c r="C36" s="1">
-        <v>3.3333333333331501E-2</v>
-      </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13">
-        <f t="shared" si="0"/>
-        <v>42037</v>
-      </c>
-      <c r="B37" s="1">
-        <v>3.3333333333333298E-2</v>
-      </c>
-      <c r="C37" s="1">
-        <v>3.4374999999998102E-2</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="13">
-        <f t="shared" si="0"/>
-        <v>42038</v>
-      </c>
-      <c r="B38" s="1">
-        <v>3.4375000000000003E-2</v>
-      </c>
-      <c r="C38" s="1">
-        <v>3.5416666666664702E-2</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13">
-        <f t="shared" si="0"/>
-        <v>42039</v>
-      </c>
-      <c r="B39" s="1">
-        <v>3.54166666666667E-2</v>
-      </c>
-      <c r="C39" s="1">
-        <v>3.64583333333314E-2</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13">
-        <f t="shared" si="0"/>
-        <v>42040</v>
-      </c>
-      <c r="B40" s="1">
-        <v>3.6458333333333301E-2</v>
-      </c>
-      <c r="C40" s="1">
-        <v>3.7499999999998E-2</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13">
-        <f t="shared" si="0"/>
-        <v>42041</v>
-      </c>
-      <c r="B41" s="1">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="C41" s="1">
-        <v>3.8541666666664601E-2</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13">
-        <f t="shared" si="0"/>
-        <v>42042</v>
-      </c>
-      <c r="B42" s="1">
-        <v>3.8541666666666703E-2</v>
-      </c>
-      <c r="C42" s="1">
-        <v>3.9583333333331201E-2</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="13">
-        <f t="shared" si="0"/>
-        <v>42043</v>
-      </c>
-      <c r="B43" s="1">
-        <v>3.9583333333333297E-2</v>
-      </c>
-      <c r="C43" s="1">
-        <v>4.0624999999997802E-2</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="13">
-        <f t="shared" si="0"/>
-        <v>42044</v>
-      </c>
-      <c r="B44" s="1">
-        <v>4.0625000000000001E-2</v>
-      </c>
-      <c r="C44" s="1">
-        <v>4.1666666666664402E-2</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13">
-        <f t="shared" si="0"/>
-        <v>42045</v>
-      </c>
-      <c r="B45" s="1">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="C45" s="1">
-        <v>4.2708333333331003E-2</v>
-      </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13">
-        <f t="shared" si="0"/>
-        <v>42046</v>
-      </c>
-      <c r="B46" s="1">
-        <v>4.27083333333333E-2</v>
-      </c>
-      <c r="C46" s="1">
-        <v>4.3749999999997603E-2</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="13">
-        <f t="shared" si="0"/>
-        <v>42047</v>
-      </c>
-      <c r="B47" s="1">
-        <v>4.3749999999999997E-2</v>
-      </c>
-      <c r="C47" s="1">
-        <v>4.4791666666664197E-2</v>
-      </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="13">
-        <f t="shared" si="0"/>
-        <v>42048</v>
-      </c>
-      <c r="B48" s="1">
-        <v>4.4791666666666702E-2</v>
-      </c>
-      <c r="C48" s="1">
-        <v>4.5833333333330797E-2</v>
-      </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="13">
-        <f t="shared" si="0"/>
-        <v>42049</v>
-      </c>
-      <c r="B49" s="1">
-        <v>4.5833333333333302E-2</v>
-      </c>
-      <c r="C49" s="1">
-        <v>4.6874999999997398E-2</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="13">
-        <f t="shared" si="0"/>
-        <v>42050</v>
-      </c>
-      <c r="B50" s="1">
-        <v>4.6875E-2</v>
-      </c>
-      <c r="C50" s="1">
-        <v>4.7916666666663998E-2</v>
-      </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="13">
-        <f t="shared" si="0"/>
-        <v>42051</v>
-      </c>
-      <c r="B51" s="1">
-        <v>4.7916666666666698E-2</v>
-      </c>
-      <c r="C51" s="1">
-        <v>4.8958333333330599E-2</v>
-      </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="13">
-        <f t="shared" si="0"/>
-        <v>42052</v>
-      </c>
-      <c r="B52" s="1">
-        <v>4.8958333333333298E-2</v>
-      </c>
-      <c r="C52" s="1">
-        <v>4.9999999999997297E-2</v>
-      </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="13">
-        <f t="shared" si="0"/>
-        <v>42053</v>
-      </c>
-      <c r="B53" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="C53" s="1">
-        <v>5.1041666666663897E-2</v>
-      </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="13">
-        <f t="shared" si="0"/>
-        <v>42054</v>
-      </c>
-      <c r="B54" s="1">
-        <v>5.10416666666667E-2</v>
-      </c>
-      <c r="C54" s="1">
-        <v>5.2083333333330498E-2</v>
-      </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="13">
-        <f t="shared" si="0"/>
-        <v>42055</v>
-      </c>
-      <c r="B55" s="1">
-        <v>5.2083333333333301E-2</v>
-      </c>
-      <c r="C55" s="1">
-        <v>5.3124999999997098E-2</v>
-      </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="13">
-        <f t="shared" si="0"/>
-        <v>42056</v>
-      </c>
-      <c r="B56" s="1">
-        <v>5.3124999999999999E-2</v>
-      </c>
-      <c r="C56" s="1">
-        <v>5.4166666666663699E-2</v>
-      </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="13">
-        <f t="shared" si="0"/>
-        <v>42057</v>
-      </c>
-      <c r="B57" s="1">
-        <v>5.4166666666666703E-2</v>
-      </c>
-      <c r="C57" s="1">
-        <v>5.5208333333330299E-2</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="13">
-        <f t="shared" si="0"/>
-        <v>42058</v>
-      </c>
-      <c r="B58" s="1">
-        <v>5.5208333333333297E-2</v>
-      </c>
-      <c r="C58" s="1">
-        <v>5.62499999999969E-2</v>
-      </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="13">
-        <f t="shared" si="0"/>
-        <v>42059</v>
-      </c>
-      <c r="B59" s="1">
-        <v>5.6250000000000001E-2</v>
-      </c>
-      <c r="C59" s="1">
-        <v>5.72916666666635E-2</v>
-      </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="13">
-        <f t="shared" si="0"/>
-        <v>42060</v>
-      </c>
-      <c r="B60" s="1">
-        <v>5.7291666666666699E-2</v>
-      </c>
-      <c r="C60" s="1">
-        <v>5.8333333333330101E-2</v>
-      </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="13">
-        <f t="shared" si="0"/>
-        <v>42061</v>
-      </c>
-      <c r="B61" s="1">
-        <v>5.83333333333333E-2</v>
-      </c>
-      <c r="C61" s="1">
-        <v>5.9374999999996701E-2</v>
-      </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="13">
-        <f t="shared" si="0"/>
-        <v>42062</v>
-      </c>
-      <c r="B62" s="1">
-        <v>5.9374999999999997E-2</v>
-      </c>
-      <c r="C62" s="1">
-        <v>6.0416666666663302E-2</v>
-      </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="13">
-        <f t="shared" si="0"/>
-        <v>42063</v>
-      </c>
-      <c r="B63" s="1">
-        <v>6.0416666666666702E-2</v>
-      </c>
-      <c r="C63" s="1">
-        <v>6.1458333333329902E-2</v>
-      </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="13">
-        <f t="shared" si="0"/>
-        <v>42064</v>
-      </c>
-      <c r="B64" s="1">
-        <v>6.1458333333333302E-2</v>
-      </c>
-      <c r="C64" s="1">
-        <v>6.2499999999996503E-2</v>
-      </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="13">
-        <f t="shared" si="0"/>
-        <v>42065</v>
-      </c>
-      <c r="B65" s="1">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C65" s="1">
-        <v>6.3541666666663096E-2</v>
-      </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="13">
-        <f t="shared" si="0"/>
-        <v>42066</v>
-      </c>
-      <c r="B66" s="1">
-        <v>6.3541666666666705E-2</v>
-      </c>
-      <c r="C66" s="1">
-        <v>6.4583333333329801E-2</v>
-      </c>
-      <c r="D66" s="8"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="13">
-        <f t="shared" si="0"/>
-        <v>42067</v>
-      </c>
-      <c r="B67" s="1">
-        <v>6.4583333333333298E-2</v>
-      </c>
-      <c r="C67" s="1">
-        <v>6.5624999999996395E-2</v>
-      </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="13">
-        <f t="shared" si="0"/>
-        <v>42068</v>
-      </c>
-      <c r="B68" s="1">
-        <v>6.5625000000000003E-2</v>
-      </c>
-      <c r="C68" s="1">
-        <v>6.6666666666663002E-2</v>
-      </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="13">
-        <f t="shared" si="0"/>
-        <v>42069</v>
-      </c>
-      <c r="B69" s="1">
-        <v>6.6666666666666693E-2</v>
-      </c>
-      <c r="C69" s="1">
-        <v>6.7708333333329596E-2</v>
-      </c>
-      <c r="D69" s="8"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="13">
-        <f t="shared" si="0"/>
-        <v>42070</v>
-      </c>
-      <c r="B70" s="1">
-        <v>6.7708333333333301E-2</v>
-      </c>
-      <c r="C70" s="1">
-        <v>6.8749999999996203E-2</v>
-      </c>
-      <c r="D70" s="8"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="2"/>
-    </row>
-    <row r="71" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="13">
-        <f t="shared" ref="A71:A134" si="1">A70+1</f>
-        <v>42071</v>
-      </c>
-      <c r="B71" s="1">
-        <v>6.8750000000000006E-2</v>
-      </c>
-      <c r="C71" s="1">
-        <v>6.9791666666662797E-2</v>
-      </c>
-      <c r="D71" s="8"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="2"/>
-    </row>
-    <row r="72" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="13">
-        <f t="shared" si="1"/>
-        <v>42072</v>
-      </c>
-      <c r="B72" s="1">
-        <v>6.9791666666666696E-2</v>
-      </c>
-      <c r="C72" s="1">
-        <v>7.0833333333329404E-2</v>
-      </c>
-      <c r="D72" s="8"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="2"/>
-    </row>
-    <row r="73" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="13">
-        <f t="shared" si="1"/>
-        <v>42073</v>
-      </c>
-      <c r="B73" s="1">
-        <v>7.0833333333333304E-2</v>
-      </c>
-      <c r="C73" s="1">
-        <v>7.1874999999995998E-2</v>
-      </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="2"/>
-    </row>
-    <row r="74" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="13">
-        <f t="shared" si="1"/>
-        <v>42074</v>
-      </c>
-      <c r="B74" s="1">
-        <v>7.1874999999999994E-2</v>
-      </c>
-      <c r="C74" s="1">
-        <v>7.2916666666662605E-2</v>
-      </c>
-      <c r="D74" s="8"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="13">
-        <f t="shared" si="1"/>
-        <v>42075</v>
-      </c>
-      <c r="B75" s="1">
-        <v>7.2916666666666699E-2</v>
-      </c>
-      <c r="C75" s="1">
-        <v>7.3958333333329199E-2</v>
-      </c>
-      <c r="D75" s="8"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="13">
-        <f t="shared" si="1"/>
-        <v>42076</v>
-      </c>
-      <c r="B76" s="1">
-        <v>7.3958333333333307E-2</v>
-      </c>
-      <c r="C76" s="1">
-        <v>7.4999999999995806E-2</v>
-      </c>
-      <c r="D76" s="8"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="13">
-        <f t="shared" si="1"/>
-        <v>42077</v>
-      </c>
-      <c r="B77" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C77" s="1">
-        <v>7.60416666666624E-2</v>
-      </c>
-      <c r="D77" s="8"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="13">
-        <f t="shared" si="1"/>
-        <v>42078</v>
-      </c>
-      <c r="B78" s="1">
-        <v>7.6041666666666702E-2</v>
-      </c>
-      <c r="C78" s="1">
-        <v>7.7083333333328993E-2</v>
-      </c>
-      <c r="D78" s="8"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="2"/>
-    </row>
-    <row r="79" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="13">
-        <f t="shared" si="1"/>
-        <v>42079</v>
-      </c>
-      <c r="B79" s="1">
-        <v>7.7083333333333295E-2</v>
-      </c>
-      <c r="C79" s="1">
-        <v>7.8124999999995698E-2</v>
-      </c>
-      <c r="D79" s="8"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="13">
-        <f t="shared" si="1"/>
-        <v>42080</v>
-      </c>
-      <c r="B80" s="1">
-        <v>7.8125E-2</v>
-      </c>
-      <c r="C80" s="1">
-        <v>7.9166666666662305E-2</v>
-      </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="13">
-        <f t="shared" si="1"/>
-        <v>42081</v>
-      </c>
-      <c r="B81" s="1">
-        <v>7.9166666666666705E-2</v>
-      </c>
-      <c r="C81" s="1">
-        <v>8.0208333333328899E-2</v>
-      </c>
-      <c r="D81" s="8"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="2"/>
-    </row>
-    <row r="82" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="13">
-        <f t="shared" si="1"/>
-        <v>42082</v>
-      </c>
-      <c r="B82" s="1">
-        <v>8.0208333333333298E-2</v>
-      </c>
-      <c r="C82" s="1">
-        <v>8.1249999999995506E-2</v>
-      </c>
-      <c r="D82" s="8"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="2"/>
-    </row>
-    <row r="83" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="13">
-        <f t="shared" si="1"/>
-        <v>42083</v>
-      </c>
-      <c r="B83" s="1">
-        <v>8.1250000000000003E-2</v>
-      </c>
-      <c r="C83" s="1">
-        <v>8.22916666666621E-2</v>
-      </c>
-      <c r="D83" s="8"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="2"/>
-    </row>
-    <row r="84" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="13">
-        <f t="shared" si="1"/>
-        <v>42084</v>
-      </c>
-      <c r="B84" s="1">
-        <v>8.2291666666666693E-2</v>
-      </c>
-      <c r="C84" s="1">
-        <v>8.3333333333328694E-2</v>
-      </c>
-      <c r="D84" s="8"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="2"/>
-    </row>
-    <row r="85" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="13">
-        <f t="shared" si="1"/>
-        <v>42085</v>
-      </c>
-      <c r="B85" s="1">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="C85" s="1">
-        <v>8.4374999999995301E-2</v>
-      </c>
-      <c r="D85" s="8"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="2"/>
-    </row>
-    <row r="86" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="13">
-        <f t="shared" si="1"/>
-        <v>42086</v>
-      </c>
-      <c r="B86" s="1">
-        <v>8.4375000000000006E-2</v>
-      </c>
-      <c r="C86" s="1">
-        <v>8.5416666666661895E-2</v>
-      </c>
-      <c r="D86" s="8"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="2"/>
-    </row>
-    <row r="87" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="13">
-        <f t="shared" si="1"/>
-        <v>42087</v>
-      </c>
-      <c r="B87" s="1">
-        <v>8.5416666666666696E-2</v>
-      </c>
-      <c r="C87" s="1">
-        <v>8.6458333333328502E-2</v>
-      </c>
-      <c r="D87" s="8"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="13">
-        <f t="shared" si="1"/>
-        <v>42088</v>
-      </c>
-      <c r="B88" s="1">
-        <v>8.6458333333333304E-2</v>
-      </c>
-      <c r="C88" s="1">
-        <v>8.7499999999995096E-2</v>
-      </c>
-      <c r="D88" s="8"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="2"/>
-    </row>
-    <row r="89" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="13">
-        <f t="shared" si="1"/>
-        <v>42089</v>
-      </c>
-      <c r="B89" s="1">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="C89" s="1">
-        <v>8.8541666666661703E-2</v>
-      </c>
-      <c r="D89" s="8"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="2"/>
-    </row>
-    <row r="90" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="13">
-        <f t="shared" si="1"/>
-        <v>42090</v>
-      </c>
-      <c r="B90" s="1">
-        <v>8.8541666666666699E-2</v>
-      </c>
-      <c r="C90" s="1">
-        <v>8.9583333333328297E-2</v>
-      </c>
-      <c r="D90" s="8"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="2"/>
-    </row>
-    <row r="91" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="13">
-        <f t="shared" si="1"/>
-        <v>42091</v>
-      </c>
-      <c r="B91" s="1">
-        <v>8.9583333333333307E-2</v>
-      </c>
-      <c r="C91" s="1">
-        <v>9.0624999999994904E-2</v>
-      </c>
-      <c r="D91" s="8"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="2"/>
-    </row>
-    <row r="92" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="13">
-        <f t="shared" si="1"/>
-        <v>42092</v>
-      </c>
-      <c r="B92" s="1">
-        <v>9.0624999999999997E-2</v>
-      </c>
-      <c r="C92" s="1">
-        <v>9.1666666666661498E-2</v>
-      </c>
-      <c r="D92" s="8"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="13">
-        <f t="shared" si="1"/>
-        <v>42093</v>
-      </c>
-      <c r="B93" s="1">
-        <v>9.1666666666666702E-2</v>
-      </c>
-      <c r="C93" s="1">
-        <v>9.2708333333328202E-2</v>
-      </c>
-      <c r="D93" s="8"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="13">
-        <f t="shared" si="1"/>
-        <v>42094</v>
-      </c>
-      <c r="B94" s="1">
-        <v>9.2708333333333295E-2</v>
-      </c>
-      <c r="C94" s="1">
-        <v>9.3749999999994796E-2</v>
-      </c>
-      <c r="D94" s="8"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="2"/>
-    </row>
-    <row r="95" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="13">
-        <f t="shared" si="1"/>
-        <v>42095</v>
-      </c>
-      <c r="B95" s="1">
-        <v>9.375E-2</v>
-      </c>
-      <c r="C95" s="1">
-        <v>9.4791666666661403E-2</v>
-      </c>
-      <c r="D95" s="8"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="2"/>
-    </row>
-    <row r="96" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="13">
-        <f t="shared" si="1"/>
-        <v>42096</v>
-      </c>
-      <c r="B96" s="1">
-        <v>9.4791666666666705E-2</v>
-      </c>
-      <c r="C96" s="1">
-        <v>9.5833333333327997E-2</v>
-      </c>
-      <c r="D96" s="8"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="2"/>
-    </row>
-    <row r="97" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="13">
-        <f t="shared" si="1"/>
-        <v>42097</v>
-      </c>
-      <c r="B97" s="1">
-        <v>9.5833333333333298E-2</v>
-      </c>
-      <c r="C97" s="1">
-        <v>9.6874999999994604E-2</v>
-      </c>
-      <c r="D97" s="8"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="13">
-        <f t="shared" si="1"/>
-        <v>42098</v>
-      </c>
-      <c r="B98" s="1">
-        <v>9.6875000000000003E-2</v>
-      </c>
-      <c r="C98" s="1">
-        <v>9.7916666666661198E-2</v>
-      </c>
-      <c r="D98" s="8"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="2"/>
-    </row>
-    <row r="99" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="13">
-        <f t="shared" si="1"/>
-        <v>42099</v>
-      </c>
-      <c r="B99" s="1">
-        <v>9.7916666666666693E-2</v>
-      </c>
-      <c r="C99" s="1">
-        <v>9.8958333333327805E-2</v>
-      </c>
-      <c r="D99" s="8"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="2"/>
-    </row>
-    <row r="100" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="13">
-        <f t="shared" si="1"/>
-        <v>42100</v>
-      </c>
-      <c r="B100" s="1">
-        <v>9.8958333333333301E-2</v>
-      </c>
-      <c r="C100" s="1">
-        <v>9.9999999999994399E-2</v>
-      </c>
-      <c r="D100" s="8"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="2"/>
-    </row>
-    <row r="101" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="13">
-        <f t="shared" si="1"/>
-        <v>42101</v>
-      </c>
-      <c r="B101" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C101" s="1">
-        <v>0.10104166666666101</v>
-      </c>
-      <c r="D101" s="8"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="2"/>
-    </row>
-    <row r="102" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="13">
-        <f t="shared" si="1"/>
-        <v>42102</v>
-      </c>
-      <c r="B102" s="1">
-        <v>0.101041666666667</v>
-      </c>
-      <c r="C102" s="1">
-        <v>0.102083333333328</v>
-      </c>
-      <c r="D102" s="8"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="2"/>
-    </row>
-    <row r="103" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="13">
-        <f t="shared" si="1"/>
-        <v>42103</v>
-      </c>
-      <c r="B103" s="1">
-        <v>0.102083333333333</v>
-      </c>
-      <c r="C103" s="1">
-        <v>0.103124999999995</v>
-      </c>
-      <c r="D103" s="8"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="2"/>
-    </row>
-    <row r="104" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="13">
-        <f t="shared" si="1"/>
-        <v>42104</v>
-      </c>
-      <c r="B104" s="1">
-        <v>0.10312499999999999</v>
-      </c>
-      <c r="C104" s="1">
-        <v>0.104166666666661</v>
-      </c>
-      <c r="D104" s="8"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="2"/>
-    </row>
-    <row r="105" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="13">
-        <f t="shared" si="1"/>
-        <v>42105</v>
-      </c>
-      <c r="B105" s="1">
-        <v>0.104166666666667</v>
-      </c>
-      <c r="C105" s="1">
-        <v>0.10520833333332801</v>
-      </c>
-      <c r="D105" s="8"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="2"/>
-    </row>
-    <row r="106" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="13">
-        <f t="shared" si="1"/>
-        <v>42106</v>
-      </c>
-      <c r="B106" s="1">
-        <v>0.105208333333333</v>
-      </c>
-      <c r="C106" s="1">
-        <v>0.106249999999994</v>
-      </c>
-      <c r="D106" s="8"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="2"/>
-    </row>
-    <row r="107" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="13">
-        <f t="shared" si="1"/>
-        <v>42107</v>
-      </c>
-      <c r="B107" s="1">
-        <v>0.10625</v>
-      </c>
-      <c r="C107" s="1">
-        <v>0.107291666666661</v>
-      </c>
-      <c r="D107" s="8"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="2"/>
-    </row>
-    <row r="108" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="13">
-        <f t="shared" si="1"/>
-        <v>42108</v>
-      </c>
-      <c r="B108" s="1">
-        <v>0.10729166666666699</v>
-      </c>
-      <c r="C108" s="1">
-        <v>0.10833333333332799</v>
-      </c>
-      <c r="D108" s="8"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="2"/>
-    </row>
-    <row r="109" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="13">
-        <f t="shared" si="1"/>
-        <v>42109</v>
-      </c>
-      <c r="B109" s="1">
-        <v>0.108333333333333</v>
-      </c>
-      <c r="C109" s="1">
-        <v>0.109374999999994</v>
-      </c>
-      <c r="D109" s="8"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="2"/>
-    </row>
-    <row r="110" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="13">
-        <f t="shared" si="1"/>
-        <v>42110</v>
-      </c>
-      <c r="B110" s="1">
-        <v>0.109375</v>
-      </c>
-      <c r="C110" s="1">
-        <v>0.110416666666661</v>
-      </c>
-      <c r="D110" s="8"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="2"/>
-    </row>
-    <row r="111" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="13">
-        <f t="shared" si="1"/>
-        <v>42111</v>
-      </c>
-      <c r="B111" s="1">
-        <v>0.110416666666667</v>
-      </c>
-      <c r="C111" s="1">
-        <v>0.111458333333327</v>
-      </c>
-      <c r="D111" s="8"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="2"/>
-    </row>
-    <row r="112" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="13">
-        <f t="shared" si="1"/>
-        <v>42112</v>
-      </c>
-      <c r="B112" s="1">
-        <v>0.11145833333333301</v>
-      </c>
-      <c r="C112" s="1">
-        <v>0.11249999999999399</v>
-      </c>
-      <c r="D112" s="8"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="2"/>
-    </row>
-    <row r="113" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="13">
-        <f t="shared" si="1"/>
-        <v>42113</v>
-      </c>
-      <c r="B113" s="1">
-        <v>0.1125</v>
-      </c>
-      <c r="C113" s="1">
-        <v>0.113541666666661</v>
-      </c>
-      <c r="D113" s="8"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="2"/>
-    </row>
-    <row r="114" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="13">
-        <f t="shared" si="1"/>
-        <v>42114</v>
-      </c>
-      <c r="B114" s="1">
-        <v>0.113541666666667</v>
-      </c>
-      <c r="C114" s="1">
-        <v>0.114583333333327</v>
-      </c>
-      <c r="D114" s="8"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="2"/>
-    </row>
-    <row r="115" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="13">
-        <f t="shared" si="1"/>
-        <v>42115</v>
-      </c>
-      <c r="B115" s="1">
-        <v>0.114583333333333</v>
-      </c>
-      <c r="C115" s="1">
-        <v>0.115624999999994</v>
-      </c>
-      <c r="D115" s="8"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="2"/>
-    </row>
-    <row r="116" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="13">
-        <f t="shared" si="1"/>
-        <v>42116</v>
-      </c>
-      <c r="B116" s="1">
-        <v>0.11562500000000001</v>
-      </c>
-      <c r="C116" s="1">
-        <v>0.11666666666665999</v>
-      </c>
-      <c r="D116" s="8"/>
-      <c r="E116" s="14"/>
-      <c r="F116" s="2"/>
-    </row>
-    <row r="117" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="13">
-        <f t="shared" si="1"/>
-        <v>42117</v>
-      </c>
-      <c r="B117" s="1">
-        <v>0.116666666666667</v>
-      </c>
-      <c r="C117" s="1">
-        <v>0.117708333333327</v>
-      </c>
-      <c r="D117" s="8"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="2"/>
-    </row>
-    <row r="118" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="13">
-        <f t="shared" si="1"/>
-        <v>42118</v>
-      </c>
-      <c r="B118" s="1">
-        <v>0.117708333333333</v>
-      </c>
-      <c r="C118" s="1">
-        <v>0.118749999999994</v>
-      </c>
-      <c r="D118" s="8"/>
-      <c r="E118" s="14"/>
-      <c r="F118" s="2"/>
-    </row>
-    <row r="119" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="13">
-        <f t="shared" si="1"/>
-        <v>42119</v>
-      </c>
-      <c r="B119" s="1">
-        <v>0.11874999999999999</v>
-      </c>
-      <c r="C119" s="1">
-        <v>0.11979166666666</v>
-      </c>
-      <c r="D119" s="8"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="2"/>
-    </row>
-    <row r="120" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="13">
-        <f t="shared" si="1"/>
-        <v>42120</v>
-      </c>
-      <c r="B120" s="1">
-        <v>0.119791666666667</v>
-      </c>
-      <c r="C120" s="1">
-        <v>0.12083333333332701</v>
-      </c>
-      <c r="D120" s="8"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="2"/>
-    </row>
-    <row r="121" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="13">
-        <f t="shared" si="1"/>
-        <v>42121</v>
-      </c>
-      <c r="B121" s="1">
-        <v>0.120833333333333</v>
-      </c>
-      <c r="C121" s="1">
-        <v>0.121874999999993</v>
-      </c>
-      <c r="D121" s="8"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="2"/>
-    </row>
-    <row r="122" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="13">
-        <f t="shared" si="1"/>
-        <v>42122</v>
-      </c>
-      <c r="B122" s="1">
-        <v>0.121875</v>
-      </c>
-      <c r="C122" s="1">
-        <v>0.12291666666666</v>
-      </c>
-      <c r="D122" s="8"/>
-      <c r="E122" s="14"/>
-      <c r="F122" s="2"/>
-    </row>
-    <row r="123" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="13">
-        <f t="shared" si="1"/>
-        <v>42123</v>
-      </c>
-      <c r="B123" s="1">
-        <v>0.12291666666666699</v>
-      </c>
-      <c r="C123" s="1">
-        <v>0.12395833333332699</v>
-      </c>
-      <c r="D123" s="8"/>
-      <c r="E123" s="14"/>
-      <c r="F123" s="2"/>
-    </row>
-    <row r="124" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="13">
-        <f t="shared" si="1"/>
-        <v>42124</v>
-      </c>
-      <c r="B124" s="1">
-        <v>0.123958333333333</v>
-      </c>
-      <c r="C124" s="1">
-        <v>0.12499999999999301</v>
-      </c>
-      <c r="D124" s="8"/>
-      <c r="E124" s="14"/>
-      <c r="F124" s="2"/>
-    </row>
-    <row r="125" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="13">
-        <f t="shared" si="1"/>
-        <v>42125</v>
-      </c>
-      <c r="B125" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="C125" s="1">
-        <v>0.12604166666666</v>
-      </c>
-      <c r="D125" s="8"/>
-      <c r="E125" s="14"/>
-      <c r="F125" s="2"/>
-    </row>
-    <row r="126" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="13">
-        <f t="shared" si="1"/>
-        <v>42126</v>
-      </c>
-      <c r="B126" s="1">
-        <v>0.126041666666667</v>
-      </c>
-      <c r="C126" s="1">
-        <v>0.127083333333327</v>
-      </c>
-      <c r="D126" s="8"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="2"/>
-    </row>
-    <row r="127" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="13">
-        <f t="shared" si="1"/>
-        <v>42127</v>
-      </c>
-      <c r="B127" s="1">
-        <v>0.12708333333333299</v>
-      </c>
-      <c r="C127" s="1">
-        <v>0.12812499999999299</v>
-      </c>
-      <c r="D127" s="8"/>
-      <c r="E127" s="14"/>
-      <c r="F127" s="2"/>
-    </row>
-    <row r="128" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="13">
-        <f t="shared" si="1"/>
-        <v>42128</v>
-      </c>
-      <c r="B128" s="1">
-        <v>0.12812499999999999</v>
-      </c>
-      <c r="C128" s="1">
-        <v>0.12916666666665999</v>
-      </c>
-      <c r="D128" s="8"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="2"/>
-    </row>
-    <row r="129" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="13">
-        <f t="shared" si="1"/>
-        <v>42129</v>
-      </c>
-      <c r="B129" s="1">
-        <v>0.12916666666666701</v>
-      </c>
-      <c r="C129" s="1">
-        <v>0.13020833333332599</v>
-      </c>
-      <c r="D129" s="8"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="2"/>
-    </row>
-    <row r="130" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="13">
-        <f t="shared" si="1"/>
-        <v>42130</v>
-      </c>
-      <c r="B130" s="1">
-        <v>0.13020833333333301</v>
-      </c>
-      <c r="C130" s="1">
-        <v>0.13124999999999301</v>
-      </c>
-      <c r="D130" s="8"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="2"/>
-    </row>
-    <row r="131" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="13">
-        <f t="shared" si="1"/>
-        <v>42131</v>
-      </c>
-      <c r="B131" s="1">
-        <v>0.13125000000000001</v>
-      </c>
-      <c r="C131" s="1">
-        <v>0.13229166666666001</v>
-      </c>
-      <c r="D131" s="8"/>
-      <c r="E131" s="14"/>
-      <c r="F131" s="2"/>
-    </row>
-    <row r="132" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="13">
-        <f t="shared" si="1"/>
-        <v>42132</v>
-      </c>
-      <c r="B132" s="1">
-        <v>0.132291666666667</v>
-      </c>
-      <c r="C132" s="1">
-        <v>0.133333333333326</v>
-      </c>
-      <c r="D132" s="8"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="2"/>
-    </row>
-    <row r="133" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="13">
-        <f t="shared" si="1"/>
-        <v>42133</v>
-      </c>
-      <c r="B133" s="1">
-        <v>0.133333333333333</v>
-      </c>
-      <c r="C133" s="1">
-        <v>0.134374999999993</v>
-      </c>
-      <c r="D133" s="8"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="2"/>
-    </row>
-    <row r="134" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="13">
-        <f t="shared" si="1"/>
-        <v>42134</v>
-      </c>
-      <c r="B134" s="1">
-        <v>0.13437499999999999</v>
-      </c>
-      <c r="C134" s="1">
-        <v>0.135416666666659</v>
-      </c>
-      <c r="D134" s="8"/>
-      <c r="E134" s="14"/>
-      <c r="F134" s="2"/>
-    </row>
-    <row r="135" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="13">
-        <f t="shared" ref="A135:A163" si="2">A134+1</f>
-        <v>42135</v>
-      </c>
-      <c r="B135" s="1">
-        <v>0.13541666666666699</v>
-      </c>
-      <c r="C135" s="1">
-        <v>0.13645833333332599</v>
-      </c>
-      <c r="D135" s="8"/>
-      <c r="E135" s="14"/>
-      <c r="F135" s="2"/>
-    </row>
-    <row r="136" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="13">
-        <f t="shared" si="2"/>
-        <v>42136</v>
-      </c>
-      <c r="B136" s="1">
-        <v>0.13645833333333299</v>
-      </c>
-      <c r="C136" s="1">
-        <v>0.13749999999999299</v>
-      </c>
-      <c r="D136" s="8"/>
-      <c r="E136" s="14"/>
-      <c r="F136" s="2"/>
-    </row>
-    <row r="137" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="13">
-        <f t="shared" si="2"/>
-        <v>42137</v>
-      </c>
-      <c r="B137" s="1">
-        <v>0.13750000000000001</v>
-      </c>
-      <c r="C137" s="1">
-        <v>0.13854166666665901</v>
-      </c>
-      <c r="D137" s="8"/>
-      <c r="E137" s="14"/>
-      <c r="F137" s="2"/>
-    </row>
-    <row r="138" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="13">
-        <f t="shared" si="2"/>
-        <v>42138</v>
-      </c>
-      <c r="B138" s="1">
-        <v>0.13854166666666701</v>
-      </c>
-      <c r="C138" s="1">
-        <v>0.13958333333332601</v>
-      </c>
-      <c r="D138" s="8"/>
-      <c r="E138" s="14"/>
-      <c r="F138" s="2"/>
-    </row>
-    <row r="139" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="13">
-        <f t="shared" si="2"/>
-        <v>42139</v>
-      </c>
-      <c r="B139" s="1">
-        <v>0.139583333333333</v>
-      </c>
-      <c r="C139" s="1">
-        <v>0.14062499999999201</v>
-      </c>
-      <c r="D139" s="8"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="2"/>
-    </row>
-    <row r="140" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="13">
-        <f t="shared" si="2"/>
-        <v>42140</v>
-      </c>
-      <c r="B140" s="1">
-        <v>0.140625</v>
-      </c>
-      <c r="C140" s="1">
-        <v>0.141666666666659</v>
-      </c>
-      <c r="D140" s="8"/>
-      <c r="E140" s="14"/>
-      <c r="F140" s="2"/>
-    </row>
-    <row r="141" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="13">
-        <f t="shared" si="2"/>
-        <v>42141</v>
-      </c>
-      <c r="B141" s="1">
-        <v>0.141666666666667</v>
-      </c>
-      <c r="C141" s="1">
-        <v>0.142708333333326</v>
-      </c>
-      <c r="D141" s="8"/>
-      <c r="E141" s="14"/>
-      <c r="F141" s="2"/>
-    </row>
-    <row r="142" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="13">
-        <f t="shared" si="2"/>
-        <v>42142</v>
-      </c>
-      <c r="B142" s="1">
-        <v>0.14270833333333299</v>
-      </c>
-      <c r="C142" s="1">
-        <v>0.143749999999992</v>
-      </c>
-      <c r="D142" s="8"/>
-      <c r="E142" s="14"/>
-      <c r="F142" s="2"/>
-    </row>
-    <row r="143" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="13">
-        <f t="shared" si="2"/>
-        <v>42143</v>
-      </c>
-      <c r="B143" s="1">
-        <v>0.14374999999999999</v>
-      </c>
-      <c r="C143" s="1">
-        <v>0.14479166666665899</v>
-      </c>
-      <c r="D143" s="8"/>
-      <c r="E143" s="14"/>
-      <c r="F143" s="2"/>
-    </row>
-    <row r="144" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="13">
-        <f t="shared" si="2"/>
-        <v>42144</v>
-      </c>
-      <c r="B144" s="1">
-        <v>0.14479166666666701</v>
-      </c>
-      <c r="C144" s="1">
-        <v>0.14583333333332499</v>
-      </c>
-      <c r="D144" s="8"/>
-      <c r="E144" s="14"/>
-      <c r="F144" s="2"/>
-    </row>
-    <row r="145" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="13">
-        <f t="shared" si="2"/>
-        <v>42145</v>
-      </c>
-      <c r="B145" s="1">
-        <v>0.14583333333333301</v>
-      </c>
-      <c r="C145" s="1">
-        <v>0.14687499999999201</v>
-      </c>
-      <c r="D145" s="8"/>
-      <c r="E145" s="14"/>
-      <c r="F145" s="2"/>
-    </row>
-    <row r="146" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="13">
-        <f t="shared" si="2"/>
-        <v>42146</v>
-      </c>
-      <c r="B146" s="1">
-        <v>0.14687500000000001</v>
-      </c>
-      <c r="C146" s="1">
-        <v>0.14791666666665901</v>
-      </c>
-      <c r="D146" s="8"/>
-      <c r="E146" s="14"/>
-      <c r="F146" s="2"/>
-    </row>
-    <row r="147" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="13">
-        <f t="shared" si="2"/>
-        <v>42147</v>
-      </c>
-      <c r="B147" s="1">
-        <v>0.147916666666667</v>
-      </c>
-      <c r="C147" s="1">
-        <v>0.148958333333325</v>
-      </c>
-      <c r="D147" s="8"/>
-      <c r="E147" s="14"/>
-      <c r="F147" s="2"/>
-    </row>
-    <row r="148" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="13">
-        <f t="shared" si="2"/>
-        <v>42148</v>
-      </c>
-      <c r="B148" s="1">
-        <v>0.148958333333333</v>
-      </c>
-      <c r="C148" s="1">
-        <v>0.149999999999992</v>
-      </c>
-      <c r="D148" s="8"/>
-      <c r="E148" s="14"/>
-      <c r="F148" s="2"/>
-    </row>
-    <row r="149" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="13">
-        <f t="shared" si="2"/>
-        <v>42149</v>
-      </c>
-      <c r="B149" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="C149" s="1">
-        <v>0.151041666666658</v>
-      </c>
-      <c r="D149" s="8"/>
-      <c r="E149" s="14"/>
-      <c r="F149" s="2"/>
-    </row>
-    <row r="150" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="13">
-        <f t="shared" si="2"/>
-        <v>42150</v>
-      </c>
-      <c r="B150" s="1">
-        <v>0.15104166666666699</v>
-      </c>
-      <c r="C150" s="1">
-        <v>0.15208333333332499</v>
-      </c>
-      <c r="D150" s="8"/>
-      <c r="E150" s="14"/>
-      <c r="F150" s="2"/>
-    </row>
-    <row r="151" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="13">
-        <f t="shared" si="2"/>
-        <v>42151</v>
-      </c>
-      <c r="B151" s="1">
-        <v>0.15208333333333299</v>
-      </c>
-      <c r="C151" s="1">
-        <v>0.15312499999999199</v>
-      </c>
-      <c r="D151" s="8"/>
-      <c r="E151" s="14"/>
-      <c r="F151" s="2"/>
-    </row>
-    <row r="152" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="13">
-        <f t="shared" si="2"/>
-        <v>42152</v>
-      </c>
-      <c r="B152" s="1">
-        <v>0.15312500000000001</v>
-      </c>
-      <c r="C152" s="1">
-        <v>0.15416666666665799</v>
-      </c>
-      <c r="D152" s="8"/>
-      <c r="E152" s="14"/>
-      <c r="F152" s="2"/>
-    </row>
-    <row r="153" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="13">
-        <f t="shared" si="2"/>
-        <v>42153</v>
-      </c>
-      <c r="B153" s="1">
-        <v>0.15416666666666701</v>
-      </c>
-      <c r="C153" s="1">
-        <v>0.15520833333332501</v>
-      </c>
-      <c r="D153" s="8"/>
-      <c r="E153" s="14"/>
-      <c r="F153" s="2"/>
-    </row>
-    <row r="154" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="13">
-        <f t="shared" si="2"/>
-        <v>42154</v>
-      </c>
-      <c r="B154" s="1">
-        <v>0.155208333333333</v>
-      </c>
-      <c r="C154" s="1">
-        <v>0.15624999999999201</v>
-      </c>
-      <c r="D154" s="8"/>
-      <c r="E154" s="14"/>
-      <c r="F154" s="2"/>
-    </row>
-    <row r="155" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="13">
-        <f t="shared" si="2"/>
-        <v>42155</v>
-      </c>
-      <c r="B155" s="1">
-        <v>0.15625</v>
-      </c>
-      <c r="C155" s="1">
-        <v>0.157291666666658</v>
-      </c>
-      <c r="D155" s="8"/>
-      <c r="E155" s="14"/>
-      <c r="F155" s="2"/>
-    </row>
-    <row r="156" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="13">
-        <f t="shared" si="2"/>
-        <v>42156</v>
-      </c>
-      <c r="B156" s="1">
-        <v>0.157291666666667</v>
-      </c>
-      <c r="C156" s="1">
-        <v>0.158333333333325</v>
-      </c>
-      <c r="D156" s="8"/>
-      <c r="E156" s="14"/>
-      <c r="F156" s="2"/>
-    </row>
-    <row r="157" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="13">
-        <f t="shared" si="2"/>
-        <v>42157</v>
-      </c>
-      <c r="B157" s="1">
-        <v>0.15833333333333299</v>
-      </c>
-      <c r="C157" s="1">
-        <v>0.159374999999991</v>
-      </c>
-      <c r="D157" s="8"/>
-      <c r="E157" s="14"/>
-      <c r="F157" s="2"/>
-    </row>
-    <row r="158" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="13">
-        <f t="shared" si="2"/>
-        <v>42158</v>
-      </c>
-      <c r="B158" s="1">
-        <v>0.15937499999999999</v>
-      </c>
-      <c r="C158" s="1">
-        <v>0.16041666666665799</v>
-      </c>
-      <c r="D158" s="8"/>
-      <c r="E158" s="14"/>
-      <c r="F158" s="2"/>
-    </row>
-    <row r="159" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="13">
-        <f t="shared" si="2"/>
-        <v>42159</v>
-      </c>
-      <c r="B159" s="1">
-        <v>0.16041666666666701</v>
-      </c>
-      <c r="C159" s="1">
-        <v>0.16145833333332499</v>
-      </c>
-      <c r="D159" s="8"/>
-      <c r="E159" s="14"/>
-      <c r="F159" s="2"/>
-    </row>
-    <row r="160" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="13">
-        <f t="shared" si="2"/>
-        <v>42160</v>
-      </c>
-      <c r="B160" s="1">
-        <v>0.16145833333333301</v>
-      </c>
-      <c r="C160" s="1">
-        <v>0.16249999999999101</v>
-      </c>
-      <c r="D160" s="8"/>
-      <c r="E160" s="14"/>
-      <c r="F160" s="2"/>
-    </row>
-    <row r="161" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="13">
-        <f t="shared" si="2"/>
-        <v>42161</v>
-      </c>
-      <c r="B161" s="1">
-        <v>0.16250000000000001</v>
-      </c>
-      <c r="C161" s="1">
-        <v>0.16354166666665801</v>
-      </c>
-      <c r="D161" s="8"/>
-      <c r="E161" s="14"/>
-      <c r="F161" s="2"/>
-    </row>
-    <row r="162" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="13">
-        <f t="shared" si="2"/>
-        <v>42162</v>
-      </c>
-      <c r="B162" s="1">
-        <v>0.163541666666667</v>
-      </c>
-      <c r="C162" s="1">
-        <v>0.16458333333332401</v>
-      </c>
-      <c r="D162" s="8"/>
-      <c r="E162" s="14"/>
-      <c r="F162" s="2"/>
-    </row>
-    <row r="163" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="13">
-        <f t="shared" si="2"/>
-        <v>42163</v>
-      </c>
-      <c r="B163" s="1">
-        <v>0.164583333333333</v>
-      </c>
-      <c r="C163" s="1">
-        <v>0.165624999999991</v>
-      </c>
-      <c r="D163" s="8"/>
-      <c r="E163" s="14"/>
-      <c r="F163" s="2"/>
-    </row>
-    <row r="164" spans="1:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="12"/>
-      <c r="B164" s="12"/>
-      <c r="C164" s="12"/>
-      <c r="D164" s="12"/>
-      <c r="F164" s="12"/>
-      <c r="G164" s="12"/>
-      <c r="H164" s="12"/>
-    </row>
-    <row r="165" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="12"/>
-      <c r="B165" s="12"/>
-      <c r="C165" s="12"/>
-      <c r="D165" s="12"/>
-      <c r="F165" s="12"/>
-      <c r="G165" s="12"/>
-      <c r="H165" s="12"/>
-    </row>
-    <row r="166" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="12"/>
-      <c r="B166" s="12"/>
-      <c r="C166" s="12"/>
-      <c r="D166" s="12"/>
-      <c r="F166" s="12"/>
-      <c r="G166" s="12"/>
-      <c r="H166" s="12"/>
-    </row>
-    <row r="167" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="12"/>
-      <c r="B167" s="12"/>
-      <c r="C167" s="12"/>
-      <c r="D167" s="12"/>
-      <c r="F167" s="12"/>
-      <c r="G167" s="12"/>
-      <c r="H167" s="12"/>
-    </row>
-    <row r="168" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="12"/>
-      <c r="B168" s="12"/>
-      <c r="C168" s="12"/>
-      <c r="D168" s="12"/>
-      <c r="F168" s="12"/>
-      <c r="G168" s="12"/>
-      <c r="H168" s="12"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A169" s="12"/>
-      <c r="B169" s="12"/>
-      <c r="C169" s="12"/>
-      <c r="D169" s="12"/>
-      <c r="F169" s="12"/>
-      <c r="G169" s="12"/>
-      <c r="H169" s="12"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A170" s="12"/>
-      <c r="B170" s="12"/>
-      <c r="C170" s="12"/>
-      <c r="D170" s="12"/>
-      <c r="F170" s="12"/>
-      <c r="G170" s="12"/>
-      <c r="H170" s="12"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A171" s="12"/>
-      <c r="B171" s="12"/>
-      <c r="C171" s="12"/>
-      <c r="D171" s="12"/>
-      <c r="F171" s="12"/>
-      <c r="G171" s="12"/>
-      <c r="H171" s="12"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A172" s="12"/>
-      <c r="B172" s="12"/>
-      <c r="C172" s="12"/>
-      <c r="D172" s="12"/>
-      <c r="F172" s="12"/>
-      <c r="G172" s="12"/>
-      <c r="H172" s="12"/>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A173" s="12"/>
-      <c r="B173" s="12"/>
-      <c r="C173" s="12"/>
-      <c r="D173" s="12"/>
-      <c r="F173" s="12"/>
-      <c r="G173" s="12"/>
-      <c r="H173" s="12"/>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A174" s="12"/>
-      <c r="B174" s="12"/>
-      <c r="C174" s="12"/>
-      <c r="D174" s="12"/>
-      <c r="F174" s="12"/>
-      <c r="G174" s="12"/>
-      <c r="H174" s="12"/>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A175" s="12"/>
-      <c r="B175" s="12"/>
-      <c r="C175" s="12"/>
-      <c r="D175" s="12"/>
-      <c r="F175" s="12"/>
-      <c r="G175" s="12"/>
-      <c r="H175" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:D3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>